<commit_message>
Updated IC working files
</commit_message>
<xml_diff>
--- a/matlab/initial_conditions/plot_field_data_regions/Initial Conditions Values.xlsx
+++ b/matlab/initial_conditions/plot_field_data_regions/Initial Conditions Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\matlab\initial_conditions\plot_field_data_regions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E7096C-B78D-435E-ACB3-79EB4DB34E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DC0431-2B95-4F60-8367-30C315A0DB68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-315" windowWidth="29040" windowHeight="15990" xr2:uid="{A180E756-AE1A-4786-A003-592D82073CEE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Var</t>
   </si>
@@ -276,13 +276,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -601,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C00405-789B-4E8B-A265-FF1BD106F53F}">
-  <dimension ref="B1:U31"/>
+  <dimension ref="B1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,29 +614,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -698,55 +698,55 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>10.4</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>10.4</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>10.4</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>10.4</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>10.4</v>
       </c>
       <c r="H3" s="6">
         <v>10.4</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>10.4</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>10.4</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="8">
         <v>6</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="8">
         <v>6</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="8">
         <v>6</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="Q3" s="8">
         <v>6</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3" s="8">
         <v>6</v>
       </c>
       <c r="S3" s="6">
         <v>6</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="8">
         <v>6</v>
       </c>
-      <c r="U3" s="9">
+      <c r="U3" s="8">
         <v>6</v>
       </c>
     </row>
@@ -754,46 +754,46 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>301.875</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>301.875</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>301.875</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>301.875</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>301.875</v>
       </c>
       <c r="H4" s="6">
         <v>301.875</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>301.875</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>301.875</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="8">
         <v>254.55269999999999</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="8">
         <v>254.55269999999999</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="8">
         <v>254.55269999999999</v>
       </c>
       <c r="Q4" s="6">
         <v>254.55269999999999</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="8">
         <v>254.55269999999999</v>
       </c>
       <c r="S4" s="6">
@@ -802,7 +802,7 @@
       <c r="T4" s="6">
         <v>366.68450000000001</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U4" s="8">
         <v>366.68450000000001</v>
       </c>
     </row>
@@ -810,13 +810,13 @@
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>254.80430000000001</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>254.80430000000001</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>254.80430000000001</v>
       </c>
       <c r="F5" s="6">
@@ -828,37 +828,37 @@
       <c r="H5" s="6">
         <v>59.573</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>59.573</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>59.573</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>233.09610000000001</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="8">
         <v>233.09610000000001</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>233.09610000000001</v>
       </c>
       <c r="Q5" s="6">
         <v>233.09610000000001</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5" s="8">
         <v>125.089</v>
       </c>
       <c r="S5" s="6">
         <v>125.089</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="8">
         <v>125.089</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="8">
         <v>125.089</v>
       </c>
     </row>
@@ -875,7 +875,7 @@
       <c r="E6" s="6">
         <v>1.6875</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>1.3163</v>
       </c>
       <c r="G6" s="6">
@@ -931,7 +931,7 @@
       <c r="E7" s="6">
         <v>7.3392999999999997</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>23.839300000000001</v>
       </c>
       <c r="G7" s="6">
@@ -978,16 +978,16 @@
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.3972</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0.3972</v>
       </c>
       <c r="E8" s="6">
         <v>0.3972</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>0.2893</v>
       </c>
       <c r="G8" s="6">
@@ -1106,109 +1106,109 @@
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
+        <f>1.25*1000/12</f>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="D10" s="9">
         <f>2.5*1000/12</f>
         <v>208.33333333333334</v>
       </c>
-      <c r="D10" s="10">
-        <f>2.5*1000/12</f>
-        <v>208.33333333333334</v>
-      </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <f t="shared" ref="E10:J10" si="2">2.5*1000/12</f>
         <v>208.33333333333334</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <f t="shared" si="2"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <f t="shared" si="2"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <f t="shared" si="2"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <f t="shared" si="2"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="J10" s="10">
-        <f t="shared" si="2"/>
-        <v>208.33333333333334</v>
+      <c r="J10" s="9">
+        <f>5*1000/12</f>
+        <v>416.66666666666669</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="9">
+        <f>1.25*1000/12</f>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="O10" s="9">
         <f>2.5*1000/12</f>
         <v>208.33333333333334</v>
       </c>
-      <c r="O10" s="10">
-        <f>2.5*1000/12</f>
-        <v>208.33333333333334</v>
-      </c>
-      <c r="P10" s="10">
+      <c r="P10" s="9">
         <f t="shared" ref="P10:U10" si="3">2.5*1000/12</f>
         <v>208.33333333333334</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="9">
         <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="9">
         <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="S10" s="10">
+      <c r="S10" s="9">
         <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="T10" s="10">
+      <c r="T10" s="9">
         <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="U10" s="10">
-        <f t="shared" si="3"/>
-        <v>208.33333333333334</v>
+      <c r="U10" s="9">
+        <f>5*1000/12</f>
+        <v>416.66666666666669</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <f>C10</f>
-        <v>208.33333333333334</v>
-      </c>
-      <c r="D11" s="11">
+        <v>104.16666666666667</v>
+      </c>
+      <c r="D11" s="10">
         <f t="shared" ref="D11:J11" si="4">D10</f>
         <v>208.33333333333334</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <f t="shared" si="4"/>
-        <v>208.33333333333334</v>
+        <v>416.66666666666669</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>31</v>
@@ -1219,37 +1219,37 @@
       <c r="M11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="10">
         <f>N10</f>
-        <v>208.33333333333334</v>
-      </c>
-      <c r="O11" s="11">
+        <v>104.16666666666667</v>
+      </c>
+      <c r="O11" s="10">
         <f t="shared" ref="O11:U11" si="5">O10</f>
         <v>208.33333333333334</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="10">
         <f t="shared" si="5"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="Q11" s="11">
+      <c r="Q11" s="10">
         <f t="shared" si="5"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="R11" s="11">
+      <c r="R11" s="10">
         <f t="shared" si="5"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="S11" s="11">
+      <c r="S11" s="10">
         <f t="shared" si="5"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="T11" s="11">
+      <c r="T11" s="10">
         <f t="shared" si="5"/>
         <v>208.33333333333334</v>
       </c>
-      <c r="U11" s="11">
+      <c r="U11" s="10">
         <f t="shared" si="5"/>
-        <v>208.33333333333334</v>
+        <v>416.66666666666669</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
@@ -1257,35 +1257,35 @@
         <v>18</v>
       </c>
       <c r="C12" s="5">
-        <f>(C22 - (C6+C7))/2</f>
+        <f t="shared" ref="C12:J12" si="6">(C22 - (C6+C7))/2</f>
         <v>7.4106999999999994</v>
       </c>
       <c r="D12" s="5">
-        <f>(D22 - (D6+D7))/2</f>
+        <f t="shared" si="6"/>
         <v>5.7142499999999998</v>
       </c>
       <c r="E12" s="5">
-        <f>(E22 - (E6+E7))/2</f>
+        <f t="shared" si="6"/>
         <v>10.946400000000001</v>
       </c>
       <c r="F12" s="5">
-        <f>(F22 - (F6+F7))/2</f>
+        <f t="shared" si="6"/>
         <v>12.868649999999999</v>
       </c>
       <c r="G12" s="5">
-        <f>(G22 - (G6+G7))/2</f>
+        <f t="shared" si="6"/>
         <v>12.868649999999999</v>
       </c>
       <c r="H12" s="5">
-        <f>(H22 - (H6+H7))/2</f>
+        <f t="shared" si="6"/>
         <v>9.1123000000000012</v>
       </c>
       <c r="I12" s="5">
-        <f>(I22 - (I6+I7))/2</f>
+        <f t="shared" si="6"/>
         <v>6.3448999999999991</v>
       </c>
       <c r="J12" s="5">
-        <f>(J22 - (J6+J7))/2</f>
+        <f t="shared" si="6"/>
         <v>32.357150000000004</v>
       </c>
       <c r="K12" s="5"/>
@@ -1294,34 +1294,34 @@
         <v>18</v>
       </c>
       <c r="N12" s="5">
-        <f t="shared" ref="K12:U12" si="6">(N22 - (N6+N7))/2</f>
+        <f t="shared" ref="N12:U12" si="7">(N22 - (N6+N7))/2</f>
         <v>12.999999999999998</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="P12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12.511950000000001</v>
       </c>
       <c r="Q12" s="6">
         <v>13.2143</v>
       </c>
       <c r="R12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.940500000000004</v>
       </c>
       <c r="S12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.2205499999999994</v>
       </c>
       <c r="T12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13.918149999999999</v>
       </c>
       <c r="U12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30.491099999999989</v>
       </c>
     </row>
@@ -1334,31 +1334,31 @@
         <v>7.4106999999999994</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" ref="D13:J13" si="7">D12</f>
+        <f t="shared" ref="D13:J13" si="8">D12</f>
         <v>5.7142499999999998</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10.946400000000001</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12.868649999999999</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12.868649999999999</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.1123000000000012</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.3448999999999991</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>32.357150000000004</v>
       </c>
       <c r="K13" s="5"/>
@@ -1367,34 +1367,34 @@
         <v>19</v>
       </c>
       <c r="N13" s="5">
-        <f t="shared" ref="N13" si="8">N12</f>
+        <f t="shared" ref="N13" si="9">N12</f>
         <v>12.999999999999998</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" ref="O13" si="9">O12</f>
+        <f t="shared" ref="O13" si="10">O12</f>
         <v>8</v>
       </c>
       <c r="P13" s="5">
-        <f t="shared" ref="P13" si="10">P12</f>
+        <f t="shared" ref="P13" si="11">P12</f>
         <v>12.511950000000001</v>
       </c>
       <c r="Q13" s="6">
         <v>21.071400000000001</v>
       </c>
       <c r="R13" s="5">
-        <f t="shared" ref="R13" si="11">R12</f>
+        <f t="shared" ref="R13" si="12">R12</f>
         <v>14.940500000000004</v>
       </c>
       <c r="S13" s="5">
-        <f t="shared" ref="S13" si="12">S12</f>
+        <f t="shared" ref="S13" si="13">S12</f>
         <v>9.2205499999999994</v>
       </c>
       <c r="T13" s="5">
-        <f t="shared" ref="T13" si="13">T12</f>
+        <f t="shared" ref="T13" si="14">T12</f>
         <v>13.918149999999999</v>
       </c>
       <c r="U13" s="5">
-        <f t="shared" ref="U13" si="14">U12</f>
+        <f t="shared" ref="U13" si="15">U12</f>
         <v>30.491099999999989</v>
       </c>
     </row>
@@ -1407,31 +1407,31 @@
         <v>0.10414</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" ref="D14:J14" si="15">(D23-D8-D9)/2</f>
+        <f t="shared" ref="D14:J14" si="16">(D23-D8-D9)/2</f>
         <v>8.7989999999999999E-2</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.21773999999999999</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.14347000000000001</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.14391999999999996</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2314249999999998</v>
       </c>
       <c r="K14" s="5"/>
@@ -1440,34 +1440,34 @@
         <v>20</v>
       </c>
       <c r="N14" s="5">
-        <f t="shared" ref="K14:U14" si="16">(N23-N8-N9)/2</f>
+        <f t="shared" ref="N14:U14" si="17">(N23-N8-N9)/2</f>
         <v>0.67596999999999985</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.29289999999999999</v>
       </c>
       <c r="P14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.43217</v>
       </c>
       <c r="Q14" s="6">
         <v>0.1129</v>
       </c>
       <c r="R14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.53115999999999997</v>
       </c>
       <c r="S14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.11282500000000001</v>
       </c>
       <c r="T14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1895</v>
       </c>
       <c r="U14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.2804399999999998</v>
       </c>
     </row>
@@ -1480,31 +1480,31 @@
         <v>0.10414</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" ref="D15:J15" si="17">D14</f>
+        <f t="shared" ref="D15:J15" si="18">D14</f>
         <v>8.7989999999999999E-2</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21773999999999999</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.14347000000000001</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.14391999999999996</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2314249999999998</v>
       </c>
       <c r="K15" s="5"/>
@@ -1513,35 +1513,35 @@
         <v>21</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" ref="N15" si="18">N14</f>
+        <f t="shared" ref="N15" si="19">N14</f>
         <v>0.67596999999999985</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" ref="O15" si="19">O14</f>
+        <f t="shared" ref="O15" si="20">O14</f>
         <v>0.29289999999999999</v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" ref="P15:Q15" si="20">P14</f>
+        <f t="shared" ref="P15:Q15" si="21">P14</f>
         <v>0.43217</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.1129</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" ref="R15" si="21">R14</f>
+        <f t="shared" ref="R15" si="22">R14</f>
         <v>0.53115999999999997</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" ref="S15" si="22">S14</f>
+        <f t="shared" ref="S15" si="23">S14</f>
         <v>0.11282500000000001</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" ref="T15" si="23">T14</f>
+        <f t="shared" ref="T15" si="24">T14</f>
         <v>0.1895</v>
       </c>
       <c r="U15" s="5">
-        <f t="shared" ref="U15" si="24">U14</f>
+        <f t="shared" ref="U15" si="25">U14</f>
         <v>1.2804399999999998</v>
       </c>
     </row>
@@ -1550,36 +1550,34 @@
         <v>22</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" ref="C16:J16" si="25">(C24 * (50/12)) / 4</f>
-        <v>2.2123958333333333</v>
+        <v>0</v>
       </c>
       <c r="D16" s="5">
-        <f>(D24 * (50/12)) / 4</f>
-        <v>2.2123958333333333</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="D16:J19" si="26">(E$24 * (50/12)) / 4</f>
         <v>9.5625</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="25"/>
-        <v>1.5208333333333335</v>
+        <f>(I$24 * (50/12)) /3</f>
+        <v>2.0277777777777781</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="25"/>
-        <v>6.354166666666667</v>
+        <f>(J$24 * (50/12)) /3</f>
+        <v>8.4722222222222232</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -1587,36 +1585,34 @@
         <v>22</v>
       </c>
       <c r="N16" s="5">
-        <f t="shared" ref="K16:U16" si="26">(N24 * (50/12)) / 4</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
+        <f t="shared" ref="N16:U16" si="27">(P24 * (50/12)) / 4</f>
         <v>9.5416666666666679</v>
       </c>
-      <c r="O16" s="5">
-        <f t="shared" si="26"/>
-        <v>9.5416666666666679</v>
-      </c>
-      <c r="P16" s="5">
-        <f t="shared" si="26"/>
-        <v>9.5416666666666679</v>
-      </c>
       <c r="Q16" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>5.1865625</v>
       </c>
       <c r="R16" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>10.1953125</v>
       </c>
       <c r="S16" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>6.0057291666666677</v>
       </c>
       <c r="T16" s="5">
-        <f t="shared" si="26"/>
-        <v>10.949270833333335</v>
+        <f>(T$24 * (50/12)) /3</f>
+        <v>14.599027777777779</v>
       </c>
       <c r="U16" s="5">
-        <f t="shared" si="26"/>
-        <v>4.0755208333333339</v>
+        <f>(U$24 * (50/12)) /3</f>
+        <v>5.4340277777777786</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
@@ -1624,36 +1620,36 @@
         <v>23</v>
       </c>
       <c r="C17" s="5">
-        <f>C16</f>
-        <v>2.2123958333333333</v>
+        <f>(C$24 * (50/12)) / 2</f>
+        <v>4.4247916666666667</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" ref="D17:J17" si="27">D16</f>
-        <v>2.2123958333333333</v>
+        <f>(D$24 * (50/12)) / 2</f>
+        <v>4.4247916666666667</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>9.5625</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="27"/>
-        <v>1.5208333333333335</v>
+        <f>(I$24 * (50/12)) / 3</f>
+        <v>2.0277777777777781</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="27"/>
-        <v>6.354166666666667</v>
+        <f>(J$24 * (50/12)) / 3</f>
+        <v>8.4722222222222232</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1661,36 +1657,36 @@
         <v>23</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" ref="N17" si="28">N16</f>
+        <f>(N$24 * (50/12)) / 2</f>
+        <v>19.083333333333336</v>
+      </c>
+      <c r="O17" s="5">
+        <f>(O$24 * (50/12)) / 2</f>
+        <v>19.083333333333336</v>
+      </c>
+      <c r="P17" s="5">
+        <f t="shared" ref="P17" si="28">P16</f>
         <v>9.5416666666666679</v>
       </c>
-      <c r="O17" s="5">
-        <f t="shared" ref="O17" si="29">O16</f>
-        <v>9.5416666666666679</v>
-      </c>
-      <c r="P17" s="5">
-        <f t="shared" ref="P17" si="30">P16</f>
-        <v>9.5416666666666679</v>
-      </c>
       <c r="Q17" s="5">
-        <f t="shared" ref="Q17" si="31">Q16</f>
+        <f t="shared" ref="Q17" si="29">Q16</f>
         <v>5.1865625</v>
       </c>
       <c r="R17" s="5">
-        <f t="shared" ref="R17" si="32">R16</f>
+        <f t="shared" ref="R17" si="30">R16</f>
         <v>10.1953125</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" ref="S17" si="33">S16</f>
+        <f t="shared" ref="S17" si="31">S16</f>
         <v>6.0057291666666677</v>
       </c>
       <c r="T17" s="5">
-        <f t="shared" ref="T17" si="34">T16</f>
-        <v>10.949270833333335</v>
+        <f>(T$24 * (50/12)) / 3</f>
+        <v>14.599027777777779</v>
       </c>
       <c r="U17" s="5">
-        <f t="shared" ref="U17" si="35">U16</f>
-        <v>4.0755208333333339</v>
+        <f>(U$24 * (50/12)) / 3</f>
+        <v>5.4340277777777786</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
@@ -1698,36 +1694,34 @@
         <v>24</v>
       </c>
       <c r="C18" s="5">
-        <f>C16</f>
-        <v>2.2123958333333333</v>
+        <v>0</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" ref="D18:J18" si="36">D16</f>
-        <v>2.2123958333333333</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>9.5625</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I18" s="5">
-        <f t="shared" si="36"/>
-        <v>1.5208333333333335</v>
+        <f>(I$24 * (50/12)) / 3</f>
+        <v>2.0277777777777781</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="36"/>
-        <v>6.354166666666667</v>
+        <f>(J$24 * (50/12)) / 3</f>
+        <v>8.4722222222222232</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1735,36 +1729,34 @@
         <v>24</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" ref="K18:U18" si="37">N16</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0</v>
+      </c>
+      <c r="P18" s="5">
+        <f t="shared" ref="N18:U18" si="32">P16</f>
         <v>9.5416666666666679</v>
       </c>
-      <c r="O18" s="5">
-        <f t="shared" si="37"/>
-        <v>9.5416666666666679</v>
-      </c>
-      <c r="P18" s="5">
-        <f t="shared" si="37"/>
-        <v>9.5416666666666679</v>
-      </c>
       <c r="Q18" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>5.1865625</v>
       </c>
       <c r="R18" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>10.1953125</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>6.0057291666666677</v>
       </c>
       <c r="T18" s="5">
-        <f t="shared" si="37"/>
-        <v>10.949270833333335</v>
+        <f>(T$24 * (50/12)) / 3</f>
+        <v>14.599027777777779</v>
       </c>
       <c r="U18" s="5">
-        <f t="shared" si="37"/>
-        <v>4.0755208333333339</v>
+        <f>(U$24 * (50/12)) / 3</f>
+        <v>5.4340277777777786</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
@@ -1772,36 +1764,34 @@
         <v>25</v>
       </c>
       <c r="C19" s="5">
-        <f>C16</f>
-        <v>2.2123958333333333</v>
+        <f>(C$24 * (50/12)) / 2</f>
+        <v>4.4247916666666667</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" ref="D19:J19" si="38">D16</f>
-        <v>2.2123958333333333</v>
+        <f>(D$24 * (50/12)) / 2</f>
+        <v>4.4247916666666667</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="38"/>
+        <f t="shared" si="26"/>
         <v>9.5625</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="38"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="38"/>
+        <f t="shared" si="26"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="38"/>
+        <f t="shared" si="26"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" si="38"/>
-        <v>1.5208333333333335</v>
+        <v>0</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="38"/>
-        <v>6.354166666666667</v>
+        <v>0</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1809,36 +1799,34 @@
         <v>25</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" ref="K19:U19" si="39">N16</f>
+        <f>(N$24 * (50/12)) / 2</f>
+        <v>19.083333333333336</v>
+      </c>
+      <c r="O19" s="5">
+        <f>(O$24 * (50/12)) / 2</f>
+        <v>19.083333333333336</v>
+      </c>
+      <c r="P19" s="5">
+        <f t="shared" ref="N19:U19" si="33">P16</f>
         <v>9.5416666666666679</v>
       </c>
-      <c r="O19" s="5">
-        <f t="shared" si="39"/>
-        <v>9.5416666666666679</v>
-      </c>
-      <c r="P19" s="5">
-        <f t="shared" si="39"/>
-        <v>9.5416666666666679</v>
-      </c>
       <c r="Q19" s="5">
-        <f t="shared" si="39"/>
+        <f t="shared" si="33"/>
         <v>5.1865625</v>
       </c>
       <c r="R19" s="5">
-        <f t="shared" si="39"/>
+        <f t="shared" si="33"/>
         <v>10.1953125</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" si="39"/>
+        <f t="shared" si="33"/>
         <v>6.0057291666666677</v>
       </c>
       <c r="T19" s="5">
-        <f t="shared" si="39"/>
-        <v>10.949270833333335</v>
+        <v>0</v>
       </c>
       <c r="U19" s="5">
-        <f t="shared" si="39"/>
-        <v>4.0755208333333339</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
@@ -1915,7 +1903,7 @@
       <c r="E22" s="1">
         <v>30.919599999999999</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <v>50.892899999999997</v>
       </c>
       <c r="G22" s="1">
@@ -1971,7 +1959,7 @@
       <c r="E23" s="1">
         <v>0.87239999999999995</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>1.054</v>
       </c>
       <c r="G23" s="1">
@@ -2018,7 +2006,7 @@
       <c r="B24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>2.1238999999999999</v>
       </c>
       <c r="D24" s="1">
@@ -2027,7 +2015,7 @@
       <c r="E24" s="1">
         <v>9.18</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <v>18.793299999999999</v>
       </c>
       <c r="G24" s="1">
@@ -2045,10 +2033,10 @@
       <c r="M24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N24" s="8">
+      <c r="N24" s="7">
         <v>9.16</v>
       </c>
-      <c r="O24" s="8">
+      <c r="O24" s="7">
         <v>9.16</v>
       </c>
       <c r="P24" s="1">
@@ -2098,14 +2086,130 @@
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
     </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.25</v>
+      </c>
+      <c r="F33">
+        <v>0.25</v>
+      </c>
+      <c r="G33">
+        <v>0.25</v>
+      </c>
+      <c r="H33">
+        <v>0.25</v>
+      </c>
+      <c r="I33">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="J33">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+      <c r="E34">
+        <v>0.25</v>
+      </c>
+      <c r="F34">
+        <v>0.25</v>
+      </c>
+      <c r="G34">
+        <v>0.25</v>
+      </c>
+      <c r="H34">
+        <v>0.25</v>
+      </c>
+      <c r="I34">
+        <v>0.33</v>
+      </c>
+      <c r="J34">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0.25</v>
+      </c>
+      <c r="F35">
+        <v>0.25</v>
+      </c>
+      <c r="G35">
+        <v>0.25</v>
+      </c>
+      <c r="H35">
+        <v>0.25</v>
+      </c>
+      <c r="I35">
+        <v>0.33</v>
+      </c>
+      <c r="J35">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36">
+        <v>0.5</v>
+      </c>
+      <c r="E36">
+        <v>0.25</v>
+      </c>
+      <c r="F36">
+        <v>0.25</v>
+      </c>
+      <c r="G36">
+        <v>0.25</v>
+      </c>
+      <c r="H36">
+        <v>0.25</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C31:E31"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="N1:U1"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Initial Conditions for 2014
</commit_message>
<xml_diff>
--- a/matlab/initial_conditions/plot_field_data_regions/Initial Conditions Values.xlsx
+++ b/matlab/initial_conditions/plot_field_data_regions/Initial Conditions Values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\matlab\initial_conditions\plot_field_data_regions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DC0431-2B95-4F60-8367-30C315A0DB68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED24544-12E3-4261-8A65-ACF46793B3BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-315" windowWidth="29040" windowHeight="15990" xr2:uid="{A180E756-AE1A-4786-A003-592D82073CEE}"/>
+    <workbookView xWindow="3750" yWindow="2910" windowWidth="21600" windowHeight="11505" xr2:uid="{A180E756-AE1A-4786-A003-592D82073CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="38">
   <si>
     <t>Var</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Black Calculated</t>
+  </si>
+  <si>
+    <t>2014 Simulation</t>
   </si>
 </sst>
 </file>
@@ -280,13 +283,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,44 +604,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C00405-789B-4E8B-A265-FF1BD106F53F}">
-  <dimension ref="B1:U36"/>
+  <dimension ref="B1:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-    </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="Y1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+    </row>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -693,8 +707,35 @@
       <c r="U2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -749,8 +790,35 @@
       <c r="U3" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="AB3" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="AD3" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="AE3" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="AF3" s="6">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -805,8 +873,35 @@
       <c r="U4" s="8">
         <v>366.68450000000001</v>
       </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>301.875</v>
+      </c>
+      <c r="Z4" s="8">
+        <v>301.875</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>301.875</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>301.875</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>301.875</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>301.875</v>
+      </c>
+      <c r="AE4" s="8">
+        <v>301.875</v>
+      </c>
+      <c r="AF4" s="8">
+        <v>301.875</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
@@ -861,8 +956,35 @@
       <c r="U5" s="8">
         <v>125.089</v>
       </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>298</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>298</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>298</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>298</v>
+      </c>
+      <c r="AC5" s="6">
+        <v>518</v>
+      </c>
+      <c r="AD5" s="6">
+        <v>64</v>
+      </c>
+      <c r="AE5" s="8">
+        <v>80</v>
+      </c>
+      <c r="AF5" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -917,8 +1039,35 @@
       <c r="U6" s="6">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>1.07</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>1.46</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="AD6" s="6">
+        <v>1.48</v>
+      </c>
+      <c r="AE6" s="6">
+        <v>5.76</v>
+      </c>
+      <c r="AF6" s="6">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -973,8 +1122,35 @@
       <c r="U7" s="6">
         <v>181.07140000000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>27.39</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>18.7</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>25</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>30</v>
+      </c>
+      <c r="AF7" s="6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1029,8 +1205,35 @@
       <c r="U8" s="6">
         <v>1.7702</v>
       </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>0.3972</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>0.3972</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>0.3972</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="AC8" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="AD8" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="AE8" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="AF8" s="6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1101,8 +1304,43 @@
         <f t="shared" si="1"/>
         <v>0.17702000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y9" s="5">
+        <f>Y8*0.1</f>
+        <v>3.9720000000000005E-2</v>
+      </c>
+      <c r="Z9" s="5">
+        <f t="shared" ref="Z9:AF9" si="2">Z8*0.1</f>
+        <v>3.9720000000000005E-2</v>
+      </c>
+      <c r="AA9" s="5">
+        <f t="shared" si="2"/>
+        <v>3.9720000000000005E-2</v>
+      </c>
+      <c r="AB9" s="5">
+        <f t="shared" si="2"/>
+        <v>2.3000000000000003E-2</v>
+      </c>
+      <c r="AC9" s="5">
+        <f t="shared" si="2"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="AD9" s="5">
+        <f t="shared" si="2"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AE9" s="5">
+        <f t="shared" si="2"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="AF9" s="5">
+        <f t="shared" si="2"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1115,23 +1353,23 @@
         <v>208.33333333333334</v>
       </c>
       <c r="E10" s="9">
-        <f t="shared" ref="E10:J10" si="2">2.5*1000/12</f>
+        <f t="shared" ref="E10:I10" si="3">2.5*1000/12</f>
         <v>208.33333333333334</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
       <c r="I10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
       <c r="J10" s="9">
@@ -1150,31 +1388,66 @@
         <v>208.33333333333334</v>
       </c>
       <c r="P10" s="9">
-        <f t="shared" ref="P10:U10" si="3">2.5*1000/12</f>
+        <f t="shared" ref="P10:T10" si="4">2.5*1000/12</f>
         <v>208.33333333333334</v>
       </c>
       <c r="Q10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
       <c r="R10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
       <c r="S10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
       <c r="T10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>208.33333333333334</v>
       </c>
       <c r="U10" s="9">
         <f>5*1000/12</f>
         <v>416.66666666666669</v>
       </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y10" s="9">
+        <f>1.25*1000/12</f>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="Z10" s="9">
+        <f>2.5*1000/12</f>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AA10" s="9">
+        <f t="shared" ref="AA10:AE10" si="5">2.5*1000/12</f>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AB10" s="9">
+        <f t="shared" si="5"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AC10" s="9">
+        <f t="shared" si="5"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AD10" s="9">
+        <f t="shared" si="5"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AE10" s="9">
+        <f t="shared" si="5"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AF10" s="9">
+        <f>5*1000/12</f>
+        <v>416.66666666666669</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1183,31 +1456,31 @@
         <v>104.16666666666667</v>
       </c>
       <c r="D11" s="10">
-        <f t="shared" ref="D11:J11" si="4">D10</f>
+        <f t="shared" ref="D11:J11" si="6">D10</f>
         <v>208.33333333333334</v>
       </c>
       <c r="E11" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>208.33333333333334</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>208.33333333333334</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>208.33333333333334</v>
       </c>
       <c r="H11" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>208.33333333333334</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>208.33333333333334</v>
       </c>
       <c r="J11" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>416.66666666666669</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -1224,68 +1497,103 @@
         <v>104.16666666666667</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11:U11" si="5">O10</f>
+        <f t="shared" ref="O11:U11" si="7">O10</f>
         <v>208.33333333333334</v>
       </c>
       <c r="P11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>208.33333333333334</v>
       </c>
       <c r="Q11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>208.33333333333334</v>
       </c>
       <c r="R11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>208.33333333333334</v>
       </c>
       <c r="S11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>208.33333333333334</v>
       </c>
       <c r="T11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>208.33333333333334</v>
       </c>
       <c r="U11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>416.66666666666669</v>
       </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y11" s="10">
+        <f>Y10</f>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="Z11" s="10">
+        <f t="shared" ref="Z11:AF11" si="8">Z10</f>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AA11" s="10">
+        <f t="shared" si="8"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AB11" s="10">
+        <f t="shared" si="8"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AC11" s="10">
+        <f t="shared" si="8"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AD11" s="10">
+        <f t="shared" si="8"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AE11" s="10">
+        <f t="shared" si="8"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="AF11" s="10">
+        <f t="shared" si="8"/>
+        <v>416.66666666666669</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" ref="C12:J12" si="6">(C22 - (C6+C7))/2</f>
+        <f t="shared" ref="C12:J12" si="9">(C22 - (C6+C7))/2</f>
         <v>7.4106999999999994</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5.7142499999999998</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10.946400000000001</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>12.868649999999999</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>12.868649999999999</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9.1123000000000012</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6.3448999999999991</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>32.357150000000004</v>
       </c>
       <c r="K12" s="5"/>
@@ -1294,38 +1602,73 @@
         <v>18</v>
       </c>
       <c r="N12" s="5">
-        <f t="shared" ref="N12:U12" si="7">(N22 - (N6+N7))/2</f>
+        <f t="shared" ref="N12:U12" si="10">(N22 - (N6+N7))/2</f>
         <v>12.999999999999998</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="P12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>12.511950000000001</v>
       </c>
       <c r="Q12" s="6">
         <v>13.2143</v>
       </c>
       <c r="R12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>14.940500000000004</v>
       </c>
       <c r="S12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>9.2205499999999994</v>
       </c>
       <c r="T12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>13.918149999999999</v>
       </c>
       <c r="U12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>30.491099999999989</v>
       </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y12" s="5">
+        <f t="shared" ref="Y12:AF12" si="11">(Y22 - (Y6+Y7))/2</f>
+        <v>8.2050000000000001</v>
+      </c>
+      <c r="Z12" s="5">
+        <f t="shared" si="11"/>
+        <v>5.835</v>
+      </c>
+      <c r="AA12" s="5">
+        <f t="shared" si="11"/>
+        <v>8.3149999999999995</v>
+      </c>
+      <c r="AB12" s="5">
+        <f t="shared" si="11"/>
+        <v>9.0749999999999993</v>
+      </c>
+      <c r="AC12" s="5">
+        <f t="shared" si="11"/>
+        <v>7.2550000000000008</v>
+      </c>
+      <c r="AD12" s="5">
+        <f t="shared" si="11"/>
+        <v>9.26</v>
+      </c>
+      <c r="AE12" s="5">
+        <f t="shared" si="11"/>
+        <v>-2.379999999999999</v>
+      </c>
+      <c r="AF12" s="5">
+        <f t="shared" si="11"/>
+        <v>27.700000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1334,31 +1677,31 @@
         <v>7.4106999999999994</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" ref="D13:J13" si="8">D12</f>
+        <f t="shared" ref="D13:J13" si="12">D12</f>
         <v>5.7142499999999998</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>10.946400000000001</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12.868649999999999</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12.868649999999999</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9.1123000000000012</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6.3448999999999991</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>32.357150000000004</v>
       </c>
       <c r="K13" s="5"/>
@@ -1367,38 +1710,73 @@
         <v>19</v>
       </c>
       <c r="N13" s="5">
-        <f t="shared" ref="N13" si="9">N12</f>
+        <f t="shared" ref="N13" si="13">N12</f>
         <v>12.999999999999998</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" ref="O13" si="10">O12</f>
+        <f t="shared" ref="O13" si="14">O12</f>
         <v>8</v>
       </c>
       <c r="P13" s="5">
-        <f t="shared" ref="P13" si="11">P12</f>
+        <f t="shared" ref="P13" si="15">P12</f>
         <v>12.511950000000001</v>
       </c>
       <c r="Q13" s="6">
         <v>21.071400000000001</v>
       </c>
       <c r="R13" s="5">
-        <f t="shared" ref="R13" si="12">R12</f>
+        <f t="shared" ref="R13" si="16">R12</f>
         <v>14.940500000000004</v>
       </c>
       <c r="S13" s="5">
-        <f t="shared" ref="S13" si="13">S12</f>
+        <f t="shared" ref="S13" si="17">S12</f>
         <v>9.2205499999999994</v>
       </c>
       <c r="T13" s="5">
-        <f t="shared" ref="T13" si="14">T12</f>
+        <f t="shared" ref="T13" si="18">T12</f>
         <v>13.918149999999999</v>
       </c>
       <c r="U13" s="5">
-        <f t="shared" ref="U13" si="15">U12</f>
+        <f t="shared" ref="U13" si="19">U12</f>
         <v>30.491099999999989</v>
       </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y13" s="5">
+        <f>Y12</f>
+        <v>8.2050000000000001</v>
+      </c>
+      <c r="Z13" s="5">
+        <f t="shared" ref="Z13:AF13" si="20">Z12</f>
+        <v>5.835</v>
+      </c>
+      <c r="AA13" s="5">
+        <f t="shared" si="20"/>
+        <v>8.3149999999999995</v>
+      </c>
+      <c r="AB13" s="5">
+        <f t="shared" si="20"/>
+        <v>9.0749999999999993</v>
+      </c>
+      <c r="AC13" s="5">
+        <f t="shared" si="20"/>
+        <v>7.2550000000000008</v>
+      </c>
+      <c r="AD13" s="5">
+        <f t="shared" si="20"/>
+        <v>9.26</v>
+      </c>
+      <c r="AE13" s="5">
+        <f t="shared" si="20"/>
+        <v>-2.379999999999999</v>
+      </c>
+      <c r="AF13" s="5">
+        <f t="shared" si="20"/>
+        <v>27.700000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1407,31 +1785,31 @@
         <v>0.10414</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" ref="D14:J14" si="16">(D23-D8-D9)/2</f>
+        <f t="shared" ref="D14:J14" si="21">(D23-D8-D9)/2</f>
         <v>8.7989999999999999E-2</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.21773999999999999</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.14347000000000001</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.14391999999999996</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.2314249999999998</v>
       </c>
       <c r="K14" s="5"/>
@@ -1440,38 +1818,73 @@
         <v>20</v>
       </c>
       <c r="N14" s="5">
-        <f t="shared" ref="N14:U14" si="17">(N23-N8-N9)/2</f>
+        <f t="shared" ref="N14:U14" si="22">(N23-N8-N9)/2</f>
         <v>0.67596999999999985</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.29289999999999999</v>
       </c>
       <c r="P14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.43217</v>
       </c>
       <c r="Q14" s="6">
         <v>0.1129</v>
       </c>
       <c r="R14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.53115999999999997</v>
       </c>
       <c r="S14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.11282500000000001</v>
       </c>
       <c r="T14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>0.1895</v>
       </c>
       <c r="U14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>1.2804399999999998</v>
       </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y14" s="5">
+        <f>(Y23-Y8-Y9)/2</f>
+        <v>9.6540000000000001E-2</v>
+      </c>
+      <c r="Z14" s="5">
+        <f t="shared" ref="Z14:AF14" si="23">(Z23-Z8-Z9)/2</f>
+        <v>5.6540000000000021E-2</v>
+      </c>
+      <c r="AA14" s="5">
+        <f t="shared" si="23"/>
+        <v>0.10654000000000001</v>
+      </c>
+      <c r="AB14" s="5">
+        <f t="shared" si="23"/>
+        <v>0.26350000000000001</v>
+      </c>
+      <c r="AC14" s="5">
+        <f t="shared" si="23"/>
+        <v>0.189</v>
+      </c>
+      <c r="AD14" s="5">
+        <f t="shared" si="23"/>
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AE14" s="5">
+        <f t="shared" si="23"/>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="AF14" s="5">
+        <f t="shared" si="23"/>
+        <v>0.66249999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1480,31 +1893,31 @@
         <v>0.10414</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" ref="D15:J15" si="18">D14</f>
+        <f t="shared" ref="D15:J15" si="24">D14</f>
         <v>8.7989999999999999E-2</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>0.21773999999999999</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>0.36788500000000002</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>0.14347000000000001</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>0.14391999999999996</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1.2314249999999998</v>
       </c>
       <c r="K15" s="5"/>
@@ -1513,39 +1926,74 @@
         <v>21</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" ref="N15" si="19">N14</f>
+        <f t="shared" ref="N15" si="25">N14</f>
         <v>0.67596999999999985</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" ref="O15" si="20">O14</f>
+        <f t="shared" ref="O15" si="26">O14</f>
         <v>0.29289999999999999</v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" ref="P15:Q15" si="21">P14</f>
+        <f t="shared" ref="P15:Q15" si="27">P14</f>
         <v>0.43217</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.1129</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" ref="R15" si="22">R14</f>
+        <f t="shared" ref="R15" si="28">R14</f>
         <v>0.53115999999999997</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" ref="S15" si="23">S14</f>
+        <f t="shared" ref="S15" si="29">S14</f>
         <v>0.11282500000000001</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" ref="T15" si="24">T14</f>
+        <f t="shared" ref="T15" si="30">T14</f>
         <v>0.1895</v>
       </c>
       <c r="U15" s="5">
-        <f t="shared" ref="U15" si="25">U14</f>
+        <f t="shared" ref="U15" si="31">U14</f>
         <v>1.2804399999999998</v>
       </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y15" s="5">
+        <f>Y14</f>
+        <v>9.6540000000000001E-2</v>
+      </c>
+      <c r="Z15" s="5">
+        <f t="shared" ref="Z15:AF15" si="32">Z14</f>
+        <v>5.6540000000000021E-2</v>
+      </c>
+      <c r="AA15" s="5">
+        <f t="shared" si="32"/>
+        <v>0.10654000000000001</v>
+      </c>
+      <c r="AB15" s="5">
+        <f t="shared" si="32"/>
+        <v>0.26350000000000001</v>
+      </c>
+      <c r="AC15" s="5">
+        <f t="shared" si="32"/>
+        <v>0.189</v>
+      </c>
+      <c r="AD15" s="5">
+        <f t="shared" si="32"/>
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AE15" s="5">
+        <f t="shared" si="32"/>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="AF15" s="5">
+        <f t="shared" si="32"/>
+        <v>0.66249999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1556,19 +2004,19 @@
         <v>0</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" ref="D16:J19" si="26">(E$24 * (50/12)) / 4</f>
+        <f t="shared" ref="E16:H19" si="33">(E$24 * (50/12)) / 4</f>
         <v>9.5625</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I16" s="5">
@@ -1591,19 +2039,19 @@
         <v>0</v>
       </c>
       <c r="P16" s="5">
-        <f t="shared" ref="N16:U16" si="27">(P24 * (50/12)) / 4</f>
+        <f t="shared" ref="P16:S16" si="34">(P24 * (50/12)) / 4</f>
         <v>9.5416666666666679</v>
       </c>
       <c r="Q16" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>5.1865625</v>
       </c>
       <c r="R16" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>10.1953125</v>
       </c>
       <c r="S16" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>6.0057291666666677</v>
       </c>
       <c r="T16" s="5">
@@ -1614,8 +2062,41 @@
         <f>(U$24 * (50/12)) /3</f>
         <v>5.4340277777777786</v>
       </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="5">
+        <f t="shared" ref="AA16:AD19" si="35">(AA$24 * (50/12)) / 4</f>
+        <v>4.354166666666667</v>
+      </c>
+      <c r="AB16" s="5">
+        <f t="shared" si="35"/>
+        <v>11.84375</v>
+      </c>
+      <c r="AC16" s="5">
+        <f t="shared" si="35"/>
+        <v>11.458333333333334</v>
+      </c>
+      <c r="AD16" s="5">
+        <f t="shared" si="35"/>
+        <v>6.135416666666667</v>
+      </c>
+      <c r="AE16" s="5">
+        <f>(AE$24 * (50/12)) /3</f>
+        <v>3.3166666666666669</v>
+      </c>
+      <c r="AF16" s="5">
+        <f>(AF$24 * (50/12)) /3</f>
+        <v>11.083333333333336</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1628,19 +2109,19 @@
         <v>4.4247916666666667</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>9.5625</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I17" s="5">
@@ -1665,19 +2146,19 @@
         <v>19.083333333333336</v>
       </c>
       <c r="P17" s="5">
-        <f t="shared" ref="P17" si="28">P16</f>
+        <f t="shared" ref="P17" si="36">P16</f>
         <v>9.5416666666666679</v>
       </c>
       <c r="Q17" s="5">
-        <f t="shared" ref="Q17" si="29">Q16</f>
+        <f t="shared" ref="Q17" si="37">Q16</f>
         <v>5.1865625</v>
       </c>
       <c r="R17" s="5">
-        <f t="shared" ref="R17" si="30">R16</f>
+        <f t="shared" ref="R17" si="38">R16</f>
         <v>10.1953125</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" ref="S17" si="31">S16</f>
+        <f t="shared" ref="S17" si="39">S16</f>
         <v>6.0057291666666677</v>
       </c>
       <c r="T17" s="5">
@@ -1688,8 +2169,43 @@
         <f>(U$24 * (50/12)) / 3</f>
         <v>5.4340277777777786</v>
       </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y17" s="5">
+        <f>(Y$24 * (50/12)) / 2</f>
+        <v>5.8958333333333339</v>
+      </c>
+      <c r="Z17" s="5">
+        <f>(Z$24 * (50/12)) / 2</f>
+        <v>5</v>
+      </c>
+      <c r="AA17" s="5">
+        <f t="shared" si="35"/>
+        <v>4.354166666666667</v>
+      </c>
+      <c r="AB17" s="5">
+        <f t="shared" si="35"/>
+        <v>11.84375</v>
+      </c>
+      <c r="AC17" s="5">
+        <f t="shared" si="35"/>
+        <v>11.458333333333334</v>
+      </c>
+      <c r="AD17" s="5">
+        <f t="shared" si="35"/>
+        <v>6.135416666666667</v>
+      </c>
+      <c r="AE17" s="5">
+        <f>(AE$24 * (50/12)) / 3</f>
+        <v>3.3166666666666669</v>
+      </c>
+      <c r="AF17" s="5">
+        <f>(AF$24 * (50/12)) / 3</f>
+        <v>11.083333333333336</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1700,19 +2216,19 @@
         <v>0</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>9.5625</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I18" s="5">
@@ -1735,19 +2251,19 @@
         <v>0</v>
       </c>
       <c r="P18" s="5">
-        <f t="shared" ref="N18:U18" si="32">P16</f>
+        <f t="shared" ref="P18:S18" si="40">P16</f>
         <v>9.5416666666666679</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>5.1865625</v>
       </c>
       <c r="R18" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>10.1953125</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>6.0057291666666677</v>
       </c>
       <c r="T18" s="5">
@@ -1758,8 +2274,41 @@
         <f>(U$24 * (50/12)) / 3</f>
         <v>5.4340277777777786</v>
       </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="5">
+        <f t="shared" si="35"/>
+        <v>4.354166666666667</v>
+      </c>
+      <c r="AB18" s="5">
+        <f t="shared" si="35"/>
+        <v>11.84375</v>
+      </c>
+      <c r="AC18" s="5">
+        <f t="shared" si="35"/>
+        <v>11.458333333333334</v>
+      </c>
+      <c r="AD18" s="5">
+        <f t="shared" si="35"/>
+        <v>6.135416666666667</v>
+      </c>
+      <c r="AE18" s="5">
+        <f>(AE$24 * (50/12)) / 3</f>
+        <v>3.3166666666666669</v>
+      </c>
+      <c r="AF18" s="5">
+        <f>(AF$24 * (50/12)) / 3</f>
+        <v>11.083333333333336</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1772,19 +2321,19 @@
         <v>4.4247916666666667</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>9.5625</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>19.576354166666668</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>6.4210416666666674</v>
       </c>
       <c r="I19" s="5">
@@ -1807,19 +2356,19 @@
         <v>19.083333333333336</v>
       </c>
       <c r="P19" s="5">
-        <f t="shared" ref="N19:U19" si="33">P16</f>
+        <f t="shared" ref="P19:S19" si="41">P16</f>
         <v>9.5416666666666679</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>5.1865625</v>
       </c>
       <c r="R19" s="5">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>10.1953125</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>6.0057291666666677</v>
       </c>
       <c r="T19" s="5">
@@ -1828,8 +2377,41 @@
       <c r="U19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y19" s="5">
+        <f>(Y$24 * (50/12)) / 2</f>
+        <v>5.8958333333333339</v>
+      </c>
+      <c r="Z19" s="5">
+        <f>(Z$24 * (50/12)) / 2</f>
+        <v>5</v>
+      </c>
+      <c r="AA19" s="5">
+        <f t="shared" si="35"/>
+        <v>4.354166666666667</v>
+      </c>
+      <c r="AB19" s="5">
+        <f t="shared" si="35"/>
+        <v>11.84375</v>
+      </c>
+      <c r="AC19" s="5">
+        <f t="shared" si="35"/>
+        <v>11.458333333333334</v>
+      </c>
+      <c r="AD19" s="5">
+        <f t="shared" si="35"/>
+        <v>6.135416666666667</v>
+      </c>
+      <c r="AE19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1886,11 +2468,39 @@
       <c r="U20" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>27</v>
       </c>
@@ -1945,8 +2555,35 @@
       <c r="U22" s="1">
         <v>245.80359999999999</v>
       </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>26</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>14</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>21</v>
+      </c>
+      <c r="AB22" s="7">
+        <v>47</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>34</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>45</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>31</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
@@ -2001,8 +2638,35 @@
       <c r="U23" s="1">
         <v>4.5080999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="X23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>29</v>
       </c>
@@ -2057,34 +2721,61 @@
       <c r="U24" s="1">
         <v>3.9125000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C28" s="12" t="s">
+      <c r="X24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y24" s="7">
+        <v>2.83</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="AB24" s="7">
+        <v>11.37</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>11</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>5.89</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>2.3879999999999999</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="C28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C29" s="13" t="s">
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="C29" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C30" s="14" t="s">
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C31" s="15" t="s">
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="C31" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
@@ -2203,7 +2894,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="Y1:AF1"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="N1:U1"/>

</xml_diff>